<commit_message>
Add unstarted state to excel
</commit_message>
<xml_diff>
--- a/excel/Timeline.xlsx
+++ b/excel/Timeline.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Source\ByWork\jpmc\ExcelForPM\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\excelcharts\ExcelForPM\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092CD76F-613E-48D0-84EF-F3CBE40667CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21096" yWindow="0" windowWidth="20160" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21096" yWindow="0" windowWidth="20160" windowHeight="17280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>User/market research</t>
   </si>
@@ -63,11 +62,14 @@
     <t>Setting the 
 scope</t>
   </si>
+  <si>
+    <t>Unstarted</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -142,7 +144,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -181,6 +183,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -242,17 +245,18 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D09A254E-F374-4E91-82B1-7524A1422930}" type="CELLRANGE">
-                      <a:rPr lang="en-HK"/>
+                    <a:fld id="{6F4F60D4-29B3-440D-98A4-837F845BBF37}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-HK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -265,28 +269,27 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-9BF2-4DB2-B45E-8F4C58ED62E1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8560850C-0949-43F3-865C-90559699F6DE}" type="CELLRANGE">
-                      <a:rPr lang="en-HK"/>
+                    <a:fld id="{D84889E8-7F20-407C-A843-4E023FB1AB04}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-HK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -299,28 +302,27 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-9BF2-4DB2-B45E-8F4C58ED62E1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{342404C4-EB68-4A72-AE10-785F81ABBD42}" type="CELLRANGE">
-                      <a:rPr lang="en-HK"/>
+                    <a:fld id="{2D7E5606-EA87-4DA8-9EF1-411D5FCFDCF1}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-HK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -333,28 +335,27 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-9BF2-4DB2-B45E-8F4C58ED62E1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4A2D07D-F1D5-407B-92D2-24DC3AD2C42E}" type="CELLRANGE">
-                      <a:rPr lang="en-HK"/>
+                    <a:fld id="{6D67E03F-425D-4ADC-B68F-281F9182E64D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-HK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -367,28 +368,27 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-9BF2-4DB2-B45E-8F4C58ED62E1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71EB919D-BDCE-4451-919A-A23B7DB40DDC}" type="CELLRANGE">
-                      <a:rPr lang="en-HK"/>
+                    <a:fld id="{8F411444-DD4C-4D96-9FD9-5CBB3B978C72}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-HK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -401,28 +401,27 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-9BF2-4DB2-B45E-8F4C58ED62E1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC21DDBB-A6FE-4BDE-8A84-AAE2BB2D552D}" type="CELLRANGE">
-                      <a:rPr lang="en-HK"/>
+                    <a:fld id="{1570CAB3-B695-4FFA-8F04-B0FCBF022813}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-HK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -435,28 +434,27 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-9BF2-4DB2-B45E-8F4C58ED62E1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD889119-F245-4DA6-B0BB-A3BB493D79AE}" type="CELLRANGE">
-                      <a:rPr lang="en-HK"/>
+                    <a:fld id="{E2401F2D-CE56-469A-9372-FCABF9BF806A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-HK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -469,28 +467,27 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-9BF2-4DB2-B45E-8F4C58ED62E1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F342F561-5DFC-45CB-ADBA-2218D82DD510}" type="CELLRANGE">
-                      <a:rPr lang="en-HK"/>
+                    <a:fld id="{26AB8F45-C5E7-4513-992F-CDD28EE7806B}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-HK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -503,12 +500,10 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-9BF2-4DB2-B45E-8F4C58ED62E1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -549,8 +544,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -583,7 +579,9 @@
                 </a:solidFill>
                 <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:softEdge rad="0"/>
+              </a:effectLst>
             </c:spPr>
           </c:errBars>
           <c:cat>
@@ -652,7 +650,10 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-9BF2-4DB2-B45E-8F4C58ED62E1}"/>
+            </c:ext>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
                 <c15:f>Sheet1!$A$2:$A$9</c15:f>
@@ -686,9 +687,6 @@
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-9BF2-4DB2-B45E-8F4C58ED62E1}"/>
-            </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
@@ -702,8 +700,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="580573088"/>
-        <c:axId val="580573480"/>
+        <c:axId val="414742448"/>
+        <c:axId val="414621184"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -799,7 +797,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-09C9-4B8F-B718-284B5A63CD14}"/>
             </c:ext>
@@ -821,6 +819,97 @@
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Setting the 
+scope</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>User/market research</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UX wireframe</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Prototype</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>UI design</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Animation</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Software architecture</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>   iOS development</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-09C9-4B8F-B718-284B5A63CD14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unstarted</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -876,16 +965,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:f>Sheet1!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
@@ -896,11 +979,6 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-09C9-4B8F-B718-284B5A63CD14}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -912,11 +990,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="580573088"/>
-        <c:axId val="580573480"/>
+        <c:axId val="414742448"/>
+        <c:axId val="414621184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="580573088"/>
+        <c:axId val="414742448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,7 +1029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="580573480"/>
+        <c:crossAx val="414621184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -959,7 +1037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="580573480"/>
+        <c:axId val="414621184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,7 +1047,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="580573088"/>
+        <c:crossAx val="414742448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -987,11 +1065,34 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1616,7 +1717,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1899,11 +2000,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1911,11 +2012,10 @@
     <col min="1" max="1" width="27.44140625" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="3.21875" customWidth="1"/>
+    <col min="4" max="5" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1928,8 +2028,11 @@
       <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
@@ -1940,8 +2043,9 @@
         <v>0</v>
       </c>
       <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1952,8 +2056,9 @@
         <v>0</v>
       </c>
       <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1964,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1975,7 +2080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1985,8 +2090,9 @@
       <c r="D6" s="6">
         <v>0</v>
       </c>
+      <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1996,8 +2102,9 @@
       <c r="D7" s="6">
         <v>0</v>
       </c>
+      <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2005,11 +2112,12 @@
         <v>15</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="6">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2017,29 +2125,34 @@
         <v>-12</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="6">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>